<commit_message>
Add Overleaf Summary spreadsheet
</commit_message>
<xml_diff>
--- a/Locations/Overleaf-Summary.xlsx
+++ b/Locations/Overleaf-Summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\Rainfall\DQ_Checks\Supporting_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\BritishRainfall\Locations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FD4D16D-0CAD-479C-8114-1072B78B8213}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F461DC-2DBE-4F40-857F-7632DD430C16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB439EB2-405F-49DB-B6E7-BA14DB012A76}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="225">
   <si>
     <t>Type</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Darlington (but notes are about Pickering)</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Readings / figures</t>
@@ -1081,7 +1078,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8786D1-7CD6-4527-B4E4-4972E5D141D2}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1157,56 +1156,56 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
         <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C5">
         <v>128</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
         <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1214,22 +1213,22 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>98</v>
       </c>
       <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>29</v>
-      </c>
-      <c r="G6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1237,154 +1236,154 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>79</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
         <v>32</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
         <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C8">
         <v>135</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
         <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C9">
         <v>186</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10">
         <v>138</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
         <v>41</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11">
         <v>202</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12">
         <v>310</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13">
         <v>123</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
@@ -1398,206 +1397,206 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14">
         <v>162</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
         <v>48</v>
-      </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15">
         <v>94</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
         <v>51</v>
-      </c>
-      <c r="F15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16">
         <v>66</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
         <v>54</v>
-      </c>
-      <c r="F16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17">
         <v>49</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
         <v>57</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>58</v>
-      </c>
-      <c r="G17" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18">
         <v>74</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" t="s">
         <v>61</v>
-      </c>
-      <c r="F18" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19">
         <v>76</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" t="s">
         <v>65</v>
-      </c>
-      <c r="F20" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21">
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" t="s">
         <v>68</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>69</v>
-      </c>
-      <c r="G21" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22">
         <v>265</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" t="s">
         <v>72</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
         <v>73</v>
-      </c>
-      <c r="F22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1605,22 +1604,22 @@
         <v>7</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23">
         <v>233</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
         <v>76</v>
-      </c>
-      <c r="F23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1628,45 +1627,45 @@
         <v>7</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24">
         <v>85</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F24" t="s">
         <v>11</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25">
         <v>12</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F25" t="s">
         <v>11</v>
       </c>
       <c r="G25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1674,45 +1673,45 @@
         <v>7</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26">
         <v>249</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F26" t="s">
         <v>11</v>
       </c>
       <c r="G26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C27">
         <v>158</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E27" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
         <v>84</v>
-      </c>
-      <c r="F27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1720,91 +1719,91 @@
         <v>7</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C28">
         <v>263</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E28" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" t="s">
         <v>87</v>
-      </c>
-      <c r="F28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29">
         <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E29" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" t="s">
         <v>90</v>
-      </c>
-      <c r="F29" t="s">
-        <v>58</v>
-      </c>
-      <c r="G29" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30">
         <v>49</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C31">
         <v>144</v>
       </c>
       <c r="D31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E31" t="s">
+        <v>92</v>
+      </c>
+      <c r="F31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" t="s">
         <v>93</v>
-      </c>
-      <c r="F31" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1812,22 +1811,22 @@
         <v>7</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C32">
         <v>108</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32" t="s">
         <v>96</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>97</v>
-      </c>
-      <c r="G32" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1835,22 +1834,22 @@
         <v>7</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C33">
         <v>143</v>
       </c>
       <c r="D33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G33" t="s">
         <v>97</v>
-      </c>
-      <c r="G33" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1858,22 +1857,22 @@
         <v>7</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C34">
         <v>145</v>
       </c>
       <c r="D34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F34" t="s">
+        <v>96</v>
+      </c>
+      <c r="G34" t="s">
         <v>97</v>
-      </c>
-      <c r="G34" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1881,91 +1880,91 @@
         <v>7</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35">
         <v>216</v>
       </c>
       <c r="D35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E35" t="s">
+        <v>101</v>
+      </c>
+      <c r="F35" t="s">
+        <v>96</v>
+      </c>
+      <c r="G35" t="s">
         <v>102</v>
-      </c>
-      <c r="F35" t="s">
-        <v>97</v>
-      </c>
-      <c r="G35" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36">
         <v>247</v>
       </c>
       <c r="D36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E36" t="s">
+        <v>103</v>
+      </c>
+      <c r="F36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" t="s">
         <v>104</v>
-      </c>
-      <c r="F36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G36" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C37">
         <v>49</v>
       </c>
       <c r="D37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F37" t="s">
         <v>11</v>
       </c>
       <c r="G37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C38">
         <v>223</v>
       </c>
       <c r="D38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E38" t="s">
+        <v>107</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" t="s">
         <v>108</v>
-      </c>
-      <c r="F38" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1973,137 +1972,137 @@
         <v>7</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C39">
         <v>54</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E39" t="s">
+        <v>110</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" t="s">
         <v>111</v>
-      </c>
-      <c r="F39" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C40">
         <v>90</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F40" t="s">
         <v>11</v>
       </c>
       <c r="G40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C41">
         <v>247</v>
       </c>
       <c r="D41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F41" t="s">
         <v>11</v>
       </c>
       <c r="G41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C42">
         <v>19</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E42" t="s">
+        <v>116</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" t="s">
         <v>117</v>
-      </c>
-      <c r="F42" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C43">
         <v>196</v>
       </c>
       <c r="D43" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" t="s">
         <v>120</v>
       </c>
-      <c r="E43" t="s">
-        <v>121</v>
-      </c>
       <c r="F43" t="s">
         <v>11</v>
       </c>
       <c r="G43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C44">
         <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F44" t="s">
         <v>11</v>
       </c>
       <c r="G44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2111,22 +2110,22 @@
         <v>7</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C45">
         <v>105</v>
       </c>
       <c r="D45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E45" t="s">
+        <v>124</v>
+      </c>
+      <c r="F45" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" t="s">
         <v>125</v>
-      </c>
-      <c r="F45" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2134,137 +2133,137 @@
         <v>7</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C46">
         <v>231</v>
       </c>
       <c r="D46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E46" t="s">
+        <v>126</v>
+      </c>
+      <c r="F46" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" t="s">
         <v>127</v>
-      </c>
-      <c r="F46" t="s">
-        <v>11</v>
-      </c>
-      <c r="G46" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C47">
         <v>196</v>
       </c>
       <c r="D47" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E47" t="s">
+        <v>129</v>
+      </c>
+      <c r="F47" t="s">
+        <v>57</v>
+      </c>
+      <c r="G47" t="s">
         <v>130</v>
-      </c>
-      <c r="F47" t="s">
-        <v>58</v>
-      </c>
-      <c r="G47" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C48">
         <v>38</v>
       </c>
       <c r="D48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E48" t="s">
+        <v>132</v>
+      </c>
+      <c r="F48" t="s">
+        <v>96</v>
+      </c>
+      <c r="G48" t="s">
         <v>133</v>
-      </c>
-      <c r="F48" t="s">
-        <v>97</v>
-      </c>
-      <c r="G48" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C49">
         <v>185</v>
       </c>
       <c r="D49" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E49" t="s">
+        <v>134</v>
+      </c>
+      <c r="F49" t="s">
+        <v>96</v>
+      </c>
+      <c r="G49" t="s">
         <v>135</v>
-      </c>
-      <c r="F49" t="s">
-        <v>97</v>
-      </c>
-      <c r="G49" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C50">
         <v>209</v>
       </c>
       <c r="D50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E50" t="s">
+        <v>136</v>
+      </c>
+      <c r="F50" t="s">
+        <v>96</v>
+      </c>
+      <c r="G50" t="s">
         <v>137</v>
-      </c>
-      <c r="F50" t="s">
-        <v>97</v>
-      </c>
-      <c r="G50" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C51">
         <v>162</v>
       </c>
       <c r="D51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F51" t="s">
         <v>11</v>
       </c>
       <c r="G51" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2272,22 +2271,22 @@
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C52">
         <v>30</v>
       </c>
       <c r="D52" t="s">
+        <v>141</v>
+      </c>
+      <c r="E52" t="s">
         <v>142</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" t="s">
         <v>143</v>
-      </c>
-      <c r="F52" t="s">
-        <v>11</v>
-      </c>
-      <c r="G52" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2295,45 +2294,45 @@
         <v>7</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C53">
         <v>176</v>
       </c>
       <c r="D53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E53" t="s">
+        <v>145</v>
+      </c>
+      <c r="F53" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" t="s">
         <v>146</v>
-      </c>
-      <c r="F53" t="s">
-        <v>11</v>
-      </c>
-      <c r="G53" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C54">
         <v>117</v>
       </c>
       <c r="D54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E54" t="s">
+        <v>148</v>
+      </c>
+      <c r="F54" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" t="s">
         <v>149</v>
-      </c>
-      <c r="F54" t="s">
-        <v>11</v>
-      </c>
-      <c r="G54" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2341,45 +2340,45 @@
         <v>7</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C55">
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E55" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F55" t="s">
         <v>11</v>
       </c>
       <c r="G55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C56">
         <v>166</v>
       </c>
       <c r="D56" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E56" t="s">
+        <v>153</v>
+      </c>
+      <c r="F56" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" t="s">
         <v>154</v>
-      </c>
-      <c r="F56" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2387,45 +2386,45 @@
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C57">
         <v>232</v>
       </c>
       <c r="D57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F57" t="s">
         <v>11</v>
       </c>
       <c r="G57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C58">
         <v>138</v>
       </c>
       <c r="D58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E58" t="s">
+        <v>158</v>
+      </c>
+      <c r="F58" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" t="s">
         <v>159</v>
-      </c>
-      <c r="F58" t="s">
-        <v>11</v>
-      </c>
-      <c r="G58" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2433,91 +2432,91 @@
         <v>7</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C59">
         <v>47</v>
       </c>
       <c r="D59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E59" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F59" t="s">
         <v>11</v>
       </c>
       <c r="G59" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C60">
         <v>69</v>
       </c>
       <c r="D60" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E60" t="s">
+        <v>126</v>
+      </c>
+      <c r="F60" t="s">
+        <v>11</v>
+      </c>
+      <c r="G60" t="s">
         <v>127</v>
-      </c>
-      <c r="F60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G60" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C61">
         <v>113</v>
       </c>
       <c r="D61" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E61" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F61" t="s">
         <v>11</v>
       </c>
       <c r="G61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C62">
         <v>138</v>
       </c>
       <c r="D62" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E62" t="s">
+        <v>165</v>
+      </c>
+      <c r="F62" t="s">
+        <v>96</v>
+      </c>
+      <c r="G62" t="s">
         <v>166</v>
-      </c>
-      <c r="F62" t="s">
-        <v>97</v>
-      </c>
-      <c r="G62" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2525,22 +2524,22 @@
         <v>7</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C63">
         <v>113</v>
       </c>
       <c r="D63" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E63" t="s">
+        <v>168</v>
+      </c>
+      <c r="F63" t="s">
+        <v>96</v>
+      </c>
+      <c r="G63" t="s">
         <v>169</v>
-      </c>
-      <c r="F63" t="s">
-        <v>97</v>
-      </c>
-      <c r="G63" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2548,22 +2547,22 @@
         <v>7</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C64">
         <v>115</v>
       </c>
       <c r="D64" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E64" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F64" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G64" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2571,91 +2570,91 @@
         <v>7</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C65">
         <v>169</v>
       </c>
       <c r="D65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E65" t="s">
+        <v>172</v>
+      </c>
+      <c r="F65" t="s">
+        <v>96</v>
+      </c>
+      <c r="G65" t="s">
         <v>173</v>
-      </c>
-      <c r="F65" t="s">
-        <v>97</v>
-      </c>
-      <c r="G65" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C66">
         <v>99</v>
       </c>
       <c r="D66" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E66" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F66" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C67">
         <v>126</v>
       </c>
       <c r="D67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F67" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C68">
         <v>230</v>
       </c>
       <c r="D68" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E68" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F68" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G68" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2663,22 +2662,22 @@
         <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C69">
         <v>43</v>
       </c>
       <c r="D69" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E69" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F69" t="s">
         <v>11</v>
       </c>
       <c r="G69" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2686,22 +2685,22 @@
         <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C70">
         <v>46</v>
       </c>
       <c r="D70" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E70" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F70" t="s">
         <v>11</v>
       </c>
       <c r="G70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2709,22 +2708,22 @@
         <v>7</v>
       </c>
       <c r="B71" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C71">
         <v>49</v>
       </c>
       <c r="D71" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E71" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F71" t="s">
         <v>11</v>
       </c>
       <c r="G71" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2732,22 +2731,22 @@
         <v>7</v>
       </c>
       <c r="B72" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C72">
         <v>54</v>
       </c>
       <c r="D72" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F72" t="s">
         <v>11</v>
       </c>
       <c r="G72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2755,22 +2754,22 @@
         <v>7</v>
       </c>
       <c r="B73" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C73">
         <v>56</v>
       </c>
       <c r="D73" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F73" t="s">
         <v>11</v>
       </c>
       <c r="G73" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2778,22 +2777,22 @@
         <v>7</v>
       </c>
       <c r="B74" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C74">
         <v>58</v>
       </c>
       <c r="D74" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E74" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F74" t="s">
         <v>11</v>
       </c>
       <c r="G74" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2801,22 +2800,22 @@
         <v>7</v>
       </c>
       <c r="B75" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C75">
         <v>60</v>
       </c>
       <c r="D75" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E75" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F75" t="s">
         <v>11</v>
       </c>
       <c r="G75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2824,22 +2823,22 @@
         <v>7</v>
       </c>
       <c r="B76" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C76">
         <v>66</v>
       </c>
       <c r="D76" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E76" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F76" t="s">
         <v>11</v>
       </c>
       <c r="G76" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2847,22 +2846,22 @@
         <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C77">
         <v>123</v>
       </c>
       <c r="D77" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E77" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F77" t="s">
         <v>11</v>
       </c>
       <c r="G77" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2870,45 +2869,45 @@
         <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C78">
         <v>126</v>
       </c>
       <c r="D78" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E78" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F78" t="s">
         <v>11</v>
       </c>
       <c r="G78" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B79" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C79">
         <v>140</v>
       </c>
       <c r="D79" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E79" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F79" t="s">
         <v>11</v>
       </c>
       <c r="G79" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2916,45 +2915,45 @@
         <v>7</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C80">
         <v>25</v>
       </c>
       <c r="D80" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E80" t="s">
+        <v>191</v>
+      </c>
+      <c r="F80" t="s">
+        <v>96</v>
+      </c>
+      <c r="G80" t="s">
         <v>192</v>
-      </c>
-      <c r="F80" t="s">
-        <v>97</v>
-      </c>
-      <c r="G80" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C81">
         <v>66</v>
       </c>
       <c r="D81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E81" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F81" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G81" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2962,160 +2961,160 @@
         <v>7</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C82">
         <v>69</v>
       </c>
       <c r="D82" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E82" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F82" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G82" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C83">
         <v>161</v>
       </c>
       <c r="D83" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F83" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G83" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C84">
         <v>329</v>
       </c>
       <c r="D84" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E84" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F84" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G84" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C85">
         <v>334</v>
       </c>
       <c r="D85" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E85" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F85" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G85" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B86" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C86">
         <v>31</v>
       </c>
       <c r="D86" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E86" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F86" t="s">
         <v>11</v>
       </c>
       <c r="G86" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B87" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C87">
         <v>36</v>
       </c>
       <c r="D87" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E87" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F87" t="s">
         <v>11</v>
       </c>
       <c r="G87" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B88" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C88">
         <v>86</v>
       </c>
       <c r="D88" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E88" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F88" t="s">
         <v>11</v>
       </c>
       <c r="G88" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3123,68 +3122,68 @@
         <v>7</v>
       </c>
       <c r="B89" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C89">
         <v>104</v>
       </c>
       <c r="D89" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E89" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F89" t="s">
         <v>11</v>
       </c>
       <c r="G89" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B90" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C90">
         <v>117</v>
       </c>
       <c r="D90" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E90" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F90" t="s">
         <v>11</v>
       </c>
       <c r="G90" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B91" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C91">
         <v>155</v>
       </c>
       <c r="D91" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E91" t="s">
+        <v>204</v>
+      </c>
+      <c r="F91" t="s">
+        <v>11</v>
+      </c>
+      <c r="G91" t="s">
         <v>205</v>
-      </c>
-      <c r="F91" t="s">
-        <v>11</v>
-      </c>
-      <c r="G91" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3192,22 +3191,22 @@
         <v>7</v>
       </c>
       <c r="B92" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C92">
         <v>199</v>
       </c>
       <c r="D92" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E92" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F92" t="s">
         <v>11</v>
       </c>
       <c r="G92" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3215,22 +3214,22 @@
         <v>7</v>
       </c>
       <c r="B93" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C93">
         <v>236</v>
       </c>
       <c r="D93" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E93" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F93" t="s">
         <v>11</v>
       </c>
       <c r="G93" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3238,22 +3237,22 @@
         <v>7</v>
       </c>
       <c r="B94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C94">
         <v>131</v>
       </c>
       <c r="D94" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E94" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F94" t="s">
         <v>11</v>
       </c>
       <c r="G94" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3261,68 +3260,68 @@
         <v>7</v>
       </c>
       <c r="B95" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C95">
         <v>135</v>
       </c>
       <c r="D95" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E95" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F95" t="s">
         <v>11</v>
       </c>
       <c r="G95" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B96" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C96">
         <v>92</v>
       </c>
       <c r="D96" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E96" t="s">
+        <v>212</v>
+      </c>
+      <c r="F96" t="s">
+        <v>11</v>
+      </c>
+      <c r="G96" t="s">
         <v>213</v>
-      </c>
-      <c r="F96" t="s">
-        <v>11</v>
-      </c>
-      <c r="G96" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B97" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C97">
         <v>80</v>
       </c>
       <c r="D97" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E97" t="s">
+        <v>215</v>
+      </c>
+      <c r="F97" t="s">
+        <v>11</v>
+      </c>
+      <c r="G97" t="s">
         <v>216</v>
-      </c>
-      <c r="F97" t="s">
-        <v>11</v>
-      </c>
-      <c r="G97" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3330,45 +3329,45 @@
         <v>7</v>
       </c>
       <c r="B98" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C98">
         <v>182</v>
       </c>
       <c r="D98" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E98" t="s">
+        <v>217</v>
+      </c>
+      <c r="F98" t="s">
+        <v>11</v>
+      </c>
+      <c r="G98" t="s">
         <v>218</v>
-      </c>
-      <c r="F98" t="s">
-        <v>11</v>
-      </c>
-      <c r="G98" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B99" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C99">
         <v>199</v>
       </c>
       <c r="D99" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E99" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F99" t="s">
         <v>11</v>
       </c>
       <c r="G99" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3376,45 +3375,45 @@
         <v>7</v>
       </c>
       <c r="B100" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C100">
         <v>48</v>
       </c>
       <c r="D100" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E100" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F100" t="s">
         <v>11</v>
       </c>
       <c r="G100" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C101">
         <v>106</v>
       </c>
       <c r="D101" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E101" t="s">
+        <v>223</v>
+      </c>
+      <c r="F101" t="s">
+        <v>11</v>
+      </c>
+      <c r="G101" t="s">
         <v>224</v>
-      </c>
-      <c r="F101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G101" t="s">
-        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>